<commit_message>
Feito correções na tradução.
</commit_message>
<xml_diff>
--- a/upload/src/MicroweberPackages/Translation/resources/lang_xlsx/pt_BR.xlsx
+++ b/upload/src/MicroweberPackages/Translation/resources/lang_xlsx/pt_BR.xlsx
@@ -8725,7 +8725,7 @@
     <t xml:space="preserve">Settings</t>
   </si>
   <si>
-    <t xml:space="preserve">Definições</t>
+    <t xml:space="preserve">Configurações</t>
   </si>
   <si>
     <t xml:space="preserve">Content is restored!</t>
@@ -17749,22 +17749,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E3062"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3050" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3062" activeCellId="0" sqref="D3062"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1475" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1487" activeCellId="0" sqref="D1487"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.53"/>
   </cols>
   <sheetData>
@@ -69825,7 +69825,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>